<commit_message>
Var pra obter o diretório do Excel.
</commit_message>
<xml_diff>
--- a/Teste.xlsx
+++ b/Teste.xlsx
@@ -345,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,6 +386,28 @@
         <v>300</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1000</v>
+      </c>
+      <c r="B4">
+        <v>2000</v>
+      </c>
+      <c r="C4">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10000</v>
+      </c>
+      <c r="B5">
+        <v>20000</v>
+      </c>
+      <c r="C5">
+        <v>30000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>